<commit_message>
Added latest orders and invoices to Bill of Materials and Expense Report
</commit_message>
<xml_diff>
--- a/Ordered Parts/Bill of Materials.xlsx
+++ b/Ordered Parts/Bill of Materials.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="144">
   <si>
     <t>Part</t>
   </si>
@@ -234,18 +234,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Soldering/Assembly</t>
-  </si>
-  <si>
-    <t>Screaming Circuits</t>
-  </si>
-  <si>
-    <t>*Just one company quote w/ 15-day lead time</t>
-  </si>
-  <si>
-    <t>https://www.screamingcircuits.com/quote</t>
-  </si>
-  <si>
     <t>Other Costs</t>
   </si>
   <si>
@@ -396,9 +384,6 @@
     <t>B002L5U7N2</t>
   </si>
   <si>
-    <t>*Quotes as low as $0.2303/PCB for cheapest manufacturing options</t>
-  </si>
-  <si>
     <t>Bullet Plugs</t>
   </si>
   <si>
@@ -463,6 +448,9 @@
   </si>
   <si>
     <t>https://www.arrow.com/en/products/irlb8748pbf/infineon-technologies-ag</t>
+  </si>
+  <si>
+    <t>40mm x 40mm Printed Circuit Board</t>
   </si>
 </sst>
 </file>
@@ -827,26 +815,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="B15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.3125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.89453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5234375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.1015625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.89453125" style="5"/>
-    <col min="8" max="8" width="9.20703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="51.20703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="5"/>
+    <col min="8" max="8" width="9.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="51.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -878,7 +866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -895,7 +883,7 @@
         <v>13</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G2" s="5">
         <f>18.95/50</f>
@@ -912,7 +900,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -945,24 +933,24 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G4" s="5">
         <f>6.97/100</f>
@@ -973,30 +961,30 @@
         <v>0.1394</v>
       </c>
       <c r="I4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G5" s="5">
         <f>8.62/200</f>
@@ -1007,30 +995,30 @@
         <v>8.6199999999999999E-2</v>
       </c>
       <c r="I5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G6" s="5">
         <v>0.10340000000000001</v>
@@ -1040,24 +1028,24 @@
         <v>0.41360000000000002</v>
       </c>
       <c r="I6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -1073,30 +1061,30 @@
         <v>0.55759999999999998</v>
       </c>
       <c r="I7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G8" s="5">
         <v>4.6100000000000002E-2</v>
@@ -1106,13 +1094,13 @@
         <v>0.18440000000000001</v>
       </c>
       <c r="I8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1120,16 +1108,16 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G9" s="5">
         <f>11.86/3</f>
@@ -1140,30 +1128,30 @@
         <v>3.9533333333333331</v>
       </c>
       <c r="I9" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G10" s="5">
         <v>2.99</v>
@@ -1173,30 +1161,30 @@
         <v>2.99</v>
       </c>
       <c r="I10" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B11">
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G11" s="9">
         <f>11.54/50</f>
@@ -1207,30 +1195,30 @@
         <v>0.6923999999999999</v>
       </c>
       <c r="I11" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D12" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
       </c>
       <c r="F12" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="G12" s="5">
         <f>11.6/100</f>
@@ -1241,13 +1229,13 @@
         <v>0.23199999999999998</v>
       </c>
       <c r="I12" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1255,16 +1243,16 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D13" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
       </c>
       <c r="F13" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G13" s="5">
         <f>((11.56*56)+(11.79*44))/100</f>
@@ -1275,16 +1263,16 @@
         <v>11.661199999999999</v>
       </c>
       <c r="I13" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1295,29 +1283,29 @@
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G14" s="5">
         <v>9.73</v>
       </c>
       <c r="H14" s="5">
-        <f t="shared" ref="H14:H25" si="2">B14*G14</f>
+        <f t="shared" ref="H14:H26" si="2">B14*G14</f>
         <v>9.73</v>
       </c>
       <c r="I14" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1350,9 +1338,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1361,13 +1349,13 @@
         <v>16</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="G16" s="9">
         <f>4.8/49</f>
@@ -1378,15 +1366,15 @@
         <v>9.7959183673469383E-2</v>
       </c>
       <c r="I16" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1395,13 +1383,13 @@
         <v>16</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E17" t="s">
         <v>8</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G17" s="9">
         <f>4.8/49</f>
@@ -1412,13 +1400,13 @@
         <v>9.7959183673469383E-2</v>
       </c>
       <c r="I17" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>25</v>
       </c>
@@ -1426,16 +1414,16 @@
         <v>1</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>24</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G18" s="13">
         <v>0.58450000000000002</v>
@@ -1445,13 +1433,13 @@
         <v>0.58450000000000002</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1484,7 +1472,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -1517,7 +1505,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1550,7 +1538,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -1583,7 +1571,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>57</v>
       </c>
@@ -1616,7 +1604,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -1649,7 +1637,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>65</v>
       </c>
@@ -1682,100 +1670,73 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="G26" s="4" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0.3871</v>
+      </c>
+      <c r="H26" s="5">
+        <f t="shared" si="2"/>
+        <v>0.3871</v>
+      </c>
+      <c r="I26" t="s">
+        <v>143</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G27" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H26" s="5">
-        <f>SUM(H2:H25)</f>
-        <v>44.830351700680268</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G27" s="4"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" t="s">
+      <c r="H27" s="5">
+        <f>SUM(H2:H26)</f>
+        <v>45.217451700680265</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" t="s">
-        <v>77</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29" t="s">
-        <v>69</v>
-      </c>
-      <c r="D29" t="s">
-        <v>70</v>
-      </c>
-      <c r="E29" t="s">
-        <v>70</v>
-      </c>
-      <c r="F29" t="s">
-        <v>70</v>
-      </c>
-      <c r="G29" s="5">
-        <v>0.64</v>
-      </c>
-      <c r="H29" s="5">
-        <f>B29*G29</f>
-        <v>0.64</v>
-      </c>
-      <c r="I29" t="s">
-        <v>125</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" t="s">
-        <v>71</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>72</v>
-      </c>
-      <c r="D30" t="s">
-        <v>70</v>
-      </c>
-      <c r="E30" t="s">
-        <v>70</v>
-      </c>
-      <c r="F30" t="s">
-        <v>70</v>
-      </c>
-      <c r="G30" s="5">
-        <v>8.6199999999999992</v>
-      </c>
-      <c r="H30" s="5">
-        <f>B30*G30</f>
-        <v>8.6199999999999992</v>
-      </c>
-      <c r="I30" t="s">
-        <v>73</v>
-      </c>
-      <c r="J30" s="2" t="s">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1790,26 +1751,25 @@
     <hyperlink ref="J22" r:id="rId8" xr:uid="{F70812B2-9C02-459F-B38C-705355029FE7}"/>
     <hyperlink ref="J24" r:id="rId9" xr:uid="{3F47DA3C-1E53-444A-8898-B9EA85FBD647}"/>
     <hyperlink ref="J25" r:id="rId10" xr:uid="{13709938-D199-4718-8973-2310F69E82EA}"/>
-    <hyperlink ref="J29" r:id="rId11" xr:uid="{47E9DD29-6C23-459A-8C66-8046B82569C9}"/>
-    <hyperlink ref="J30" r:id="rId12" xr:uid="{05E89BBA-B962-4888-A808-98D3B9DC0FBE}"/>
-    <hyperlink ref="A34" r:id="rId13" xr:uid="{9308F7BC-A83E-47C6-82E4-B9074942D108}"/>
-    <hyperlink ref="J6" r:id="rId14" xr:uid="{97C57276-2433-4923-8B77-CF1D09F8B548}"/>
-    <hyperlink ref="J7" r:id="rId15" xr:uid="{FC24FC01-0AA7-4D5B-BEA8-DAA6380AC073}"/>
-    <hyperlink ref="J8" r:id="rId16" xr:uid="{384DB0BE-F1AE-4448-80D7-0387BA330343}"/>
-    <hyperlink ref="J4" r:id="rId17" xr:uid="{E60A837F-D0CD-4E15-8F80-70CC3A0226A6}"/>
-    <hyperlink ref="J5" r:id="rId18" xr:uid="{4A829B53-4217-4F26-89B4-F106E6B544CD}"/>
-    <hyperlink ref="J14" r:id="rId19" xr:uid="{305F8F85-0874-4D1F-9E8A-6D0403800691}"/>
-    <hyperlink ref="K13" r:id="rId20" xr:uid="{E0DF6966-BBD6-4D0C-B6F6-D79BAA6169DB}"/>
-    <hyperlink ref="J9" r:id="rId21" xr:uid="{9DC153CF-6A36-4F67-AFC5-22DD9E35702B}"/>
-    <hyperlink ref="J10" r:id="rId22" xr:uid="{AEFCF35C-6C14-479F-9C9D-A9454FACE026}"/>
-    <hyperlink ref="J13" r:id="rId23" xr:uid="{AA52E67F-B095-4E7F-9662-B6B8C8564EF9}"/>
-    <hyperlink ref="J17" r:id="rId24" xr:uid="{4A1380DF-B3F7-4272-8054-E7C4BBA79028}"/>
-    <hyperlink ref="J16" r:id="rId25" xr:uid="{8C9B92D8-2E44-4B6A-B72A-0A081445CCF4}"/>
-    <hyperlink ref="J11" r:id="rId26" xr:uid="{3FB67847-D385-4555-A810-A1F070CC4594}"/>
-    <hyperlink ref="J12" r:id="rId27" xr:uid="{5A506C84-4FD5-4C15-9819-9ADA9D37E63C}"/>
-    <hyperlink ref="J18" r:id="rId28" xr:uid="{66DCDBD3-0A17-4F25-A19C-055A4209733C}"/>
+    <hyperlink ref="A35" r:id="rId11" xr:uid="{9308F7BC-A83E-47C6-82E4-B9074942D108}"/>
+    <hyperlink ref="J6" r:id="rId12" xr:uid="{97C57276-2433-4923-8B77-CF1D09F8B548}"/>
+    <hyperlink ref="J7" r:id="rId13" xr:uid="{FC24FC01-0AA7-4D5B-BEA8-DAA6380AC073}"/>
+    <hyperlink ref="J8" r:id="rId14" xr:uid="{384DB0BE-F1AE-4448-80D7-0387BA330343}"/>
+    <hyperlink ref="J4" r:id="rId15" xr:uid="{E60A837F-D0CD-4E15-8F80-70CC3A0226A6}"/>
+    <hyperlink ref="J5" r:id="rId16" xr:uid="{4A829B53-4217-4F26-89B4-F106E6B544CD}"/>
+    <hyperlink ref="J14" r:id="rId17" xr:uid="{305F8F85-0874-4D1F-9E8A-6D0403800691}"/>
+    <hyperlink ref="K13" r:id="rId18" xr:uid="{E0DF6966-BBD6-4D0C-B6F6-D79BAA6169DB}"/>
+    <hyperlink ref="J9" r:id="rId19" xr:uid="{9DC153CF-6A36-4F67-AFC5-22DD9E35702B}"/>
+    <hyperlink ref="J10" r:id="rId20" xr:uid="{AEFCF35C-6C14-479F-9C9D-A9454FACE026}"/>
+    <hyperlink ref="J13" r:id="rId21" xr:uid="{AA52E67F-B095-4E7F-9662-B6B8C8564EF9}"/>
+    <hyperlink ref="J17" r:id="rId22" xr:uid="{4A1380DF-B3F7-4272-8054-E7C4BBA79028}"/>
+    <hyperlink ref="J16" r:id="rId23" xr:uid="{8C9B92D8-2E44-4B6A-B72A-0A081445CCF4}"/>
+    <hyperlink ref="J11" r:id="rId24" xr:uid="{3FB67847-D385-4555-A810-A1F070CC4594}"/>
+    <hyperlink ref="J12" r:id="rId25" xr:uid="{5A506C84-4FD5-4C15-9819-9ADA9D37E63C}"/>
+    <hyperlink ref="J18" r:id="rId26" xr:uid="{66DCDBD3-0A17-4F25-A19C-055A4209733C}"/>
+    <hyperlink ref="J26" r:id="rId27" xr:uid="{DEB2DF39-759A-4E16-A9AB-E96ECF63A544}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId29"/>
+  <pageSetup orientation="portrait" r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new power adapter to bill of materials to replace old faulty supply
</commit_message>
<xml_diff>
--- a/Ordered Parts/Bill of Materials.xlsx
+++ b/Ordered Parts/Bill of Materials.xlsx
@@ -1,8 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803EFA5C-5C1C-488F-9ADA-FDBA02B04063}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11508" windowHeight="8796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,21 +76,6 @@
     <t>12V Power Supply</t>
   </si>
   <si>
-    <t>LEDMO</t>
-  </si>
-  <si>
-    <t>LED908</t>
-  </si>
-  <si>
-    <t>B01461MOGQ</t>
-  </si>
-  <si>
-    <t>12V, 5A, 60W, AC/DC Power Supply</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/LEDMO-Power-Supply-Transformers-Adapter/dp/B01461MOGQ/ref=sr_1_1?ie=UTF8&amp;qid=1516375270&amp;sr=8-1&amp;keywords=B01461MOGQ</t>
-  </si>
-  <si>
     <t>Brushless Motor</t>
   </si>
   <si>
@@ -451,6 +437,21 @@
   </si>
   <si>
     <t>40mm x 40mm Printed Circuit Board</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B00DKSI0S8/ref=ox_sc_act_title_1?smid=AAF37WJS3P6BT&amp;psc=1</t>
+  </si>
+  <si>
+    <t>LE Power Adapter, Transformers, Power Supply For LED Strip, Output 12V DC, 3A Max, 36 Watt Max, UL Listed</t>
+  </si>
+  <si>
+    <t>5000028-US</t>
+  </si>
+  <si>
+    <t>Lighting EVER</t>
+  </si>
+  <si>
+    <t>B00DKSI0S8</t>
   </si>
 </sst>
 </file>
@@ -817,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -874,16 +875,16 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G2" s="5">
         <f>18.95/50</f>
@@ -894,10 +895,10 @@
         <v>0.75800000000000001</v>
       </c>
       <c r="I2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -908,16 +909,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>143</v>
       </c>
       <c r="G3" s="5">
         <v>9.99</v>
@@ -927,30 +928,30 @@
         <v>9.99</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>140</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>22</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G4" s="5">
         <f>6.97/100</f>
@@ -961,30 +962,30 @@
         <v>0.1394</v>
       </c>
       <c r="I4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G5" s="5">
         <f>8.62/200</f>
@@ -995,30 +996,30 @@
         <v>8.6199999999999999E-2</v>
       </c>
       <c r="I5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G6" s="5">
         <v>0.10340000000000001</v>
@@ -1028,24 +1029,24 @@
         <v>0.41360000000000002</v>
       </c>
       <c r="I6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D7" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -1061,30 +1062,30 @@
         <v>0.55759999999999998</v>
       </c>
       <c r="I7" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D8" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G8" s="5">
         <v>4.6100000000000002E-2</v>
@@ -1094,10 +1095,10 @@
         <v>0.18440000000000001</v>
       </c>
       <c r="I8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -1108,16 +1109,16 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="G9" s="5">
         <f>11.86/3</f>
@@ -1128,30 +1129,30 @@
         <v>3.9533333333333331</v>
       </c>
       <c r="I9" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="G10" s="5">
         <v>2.99</v>
@@ -1161,30 +1162,30 @@
         <v>2.99</v>
       </c>
       <c r="I10" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B11">
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="G11" s="9">
         <f>11.54/50</f>
@@ -1195,30 +1196,30 @@
         <v>0.6923999999999999</v>
       </c>
       <c r="I11" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D12" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
       </c>
       <c r="F12" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="G12" s="5">
         <f>11.6/100</f>
@@ -1229,30 +1230,30 @@
         <v>0.23199999999999998</v>
       </c>
       <c r="I12" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
       </c>
       <c r="F13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G13" s="5">
         <f>((11.56*56)+(11.79*44))/100</f>
@@ -1263,13 +1264,13 @@
         <v>11.661199999999999</v>
       </c>
       <c r="I13" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1283,13 +1284,13 @@
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G14" s="5">
         <v>9.73</v>
@@ -1299,15 +1300,15 @@
         <v>9.73</v>
       </c>
       <c r="I14" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1316,13 +1317,13 @@
         <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G15" s="5">
         <v>0.01</v>
@@ -1332,15 +1333,15 @@
         <v>0.01</v>
       </c>
       <c r="I15" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1349,13 +1350,13 @@
         <v>16</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G16" s="9">
         <f>4.8/49</f>
@@ -1366,15 +1367,15 @@
         <v>9.7959183673469383E-2</v>
       </c>
       <c r="I16" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1383,13 +1384,13 @@
         <v>16</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E17" t="s">
         <v>8</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G17" s="9">
         <f>4.8/49</f>
@@ -1400,30 +1401,30 @@
         <v>9.7959183673469383E-2</v>
       </c>
       <c r="I17" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B18" s="11">
         <v>1</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="G18" s="13">
         <v>0.58450000000000002</v>
@@ -1433,30 +1434,30 @@
         <v>0.58450000000000002</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E19" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G19" s="5">
         <v>0.90280000000000005</v>
@@ -1466,30 +1467,30 @@
         <v>0.90280000000000005</v>
       </c>
       <c r="I19" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E20" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G20" s="5">
         <v>0.53400000000000003</v>
@@ -1499,30 +1500,30 @@
         <v>0.53400000000000003</v>
       </c>
       <c r="I20" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E21" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G21" s="5">
         <v>0.63229999999999997</v>
@@ -1532,30 +1533,30 @@
         <v>0.63229999999999997</v>
       </c>
       <c r="I21" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B22">
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E22" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G22" s="5">
         <v>3.0300000000000001E-2</v>
@@ -1565,30 +1566,30 @@
         <v>0.30299999999999999</v>
       </c>
       <c r="I22" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B23">
         <v>2</v>
       </c>
       <c r="C23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="E23" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G23" s="5">
         <v>3.8100000000000002E-2</v>
@@ -1598,30 +1599,30 @@
         <v>7.6200000000000004E-2</v>
       </c>
       <c r="I23" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E24" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G24" s="5">
         <v>7.5899999999999995E-2</v>
@@ -1631,30 +1632,30 @@
         <v>7.5899999999999995E-2</v>
       </c>
       <c r="I24" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B25">
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E25" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G25" s="5">
         <v>6.3799999999999996E-2</v>
@@ -1664,30 +1665,30 @@
         <v>0.12759999999999999</v>
       </c>
       <c r="I25" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E26" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G26" s="5">
         <v>0.3871</v>
@@ -1697,15 +1698,15 @@
         <v>0.3871</v>
       </c>
       <c r="I26" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G27" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H27" s="5">
         <f>SUM(H2:H26)</f>
@@ -1714,13 +1715,13 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -1731,43 +1732,43 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J3" r:id="rId1" xr:uid="{0CCFEB8D-3AF5-4B14-8755-C7F57E844E44}"/>
-    <hyperlink ref="J19" r:id="rId2" xr:uid="{5EB9FB3D-22AD-47DC-B125-539430A9CC29}"/>
-    <hyperlink ref="J15" r:id="rId3" xr:uid="{53BAB52E-738A-40FD-AE11-30F4B5C07642}"/>
-    <hyperlink ref="J20" r:id="rId4" xr:uid="{D254588B-7BF2-4663-B764-31CEE1702B72}"/>
-    <hyperlink ref="J21" r:id="rId5" xr:uid="{97844978-768D-4AF2-9FC1-EA6B6AEA91A7}"/>
-    <hyperlink ref="J2" r:id="rId6" xr:uid="{A783C18C-5336-47D4-B91E-5A0D50EFD847}"/>
-    <hyperlink ref="J23" r:id="rId7" xr:uid="{DA2D5093-8FE6-45A4-BA10-918A48B82B08}"/>
-    <hyperlink ref="J22" r:id="rId8" xr:uid="{F70812B2-9C02-459F-B38C-705355029FE7}"/>
-    <hyperlink ref="J24" r:id="rId9" xr:uid="{3F47DA3C-1E53-444A-8898-B9EA85FBD647}"/>
-    <hyperlink ref="J25" r:id="rId10" xr:uid="{13709938-D199-4718-8973-2310F69E82EA}"/>
-    <hyperlink ref="A35" r:id="rId11" xr:uid="{9308F7BC-A83E-47C6-82E4-B9074942D108}"/>
-    <hyperlink ref="J6" r:id="rId12" xr:uid="{97C57276-2433-4923-8B77-CF1D09F8B548}"/>
-    <hyperlink ref="J7" r:id="rId13" xr:uid="{FC24FC01-0AA7-4D5B-BEA8-DAA6380AC073}"/>
-    <hyperlink ref="J8" r:id="rId14" xr:uid="{384DB0BE-F1AE-4448-80D7-0387BA330343}"/>
-    <hyperlink ref="J4" r:id="rId15" xr:uid="{E60A837F-D0CD-4E15-8F80-70CC3A0226A6}"/>
-    <hyperlink ref="J5" r:id="rId16" xr:uid="{4A829B53-4217-4F26-89B4-F106E6B544CD}"/>
-    <hyperlink ref="J14" r:id="rId17" xr:uid="{305F8F85-0874-4D1F-9E8A-6D0403800691}"/>
-    <hyperlink ref="K13" r:id="rId18" xr:uid="{E0DF6966-BBD6-4D0C-B6F6-D79BAA6169DB}"/>
-    <hyperlink ref="J9" r:id="rId19" xr:uid="{9DC153CF-6A36-4F67-AFC5-22DD9E35702B}"/>
-    <hyperlink ref="J10" r:id="rId20" xr:uid="{AEFCF35C-6C14-479F-9C9D-A9454FACE026}"/>
-    <hyperlink ref="J13" r:id="rId21" xr:uid="{AA52E67F-B095-4E7F-9662-B6B8C8564EF9}"/>
-    <hyperlink ref="J17" r:id="rId22" xr:uid="{4A1380DF-B3F7-4272-8054-E7C4BBA79028}"/>
-    <hyperlink ref="J16" r:id="rId23" xr:uid="{8C9B92D8-2E44-4B6A-B72A-0A081445CCF4}"/>
-    <hyperlink ref="J11" r:id="rId24" xr:uid="{3FB67847-D385-4555-A810-A1F070CC4594}"/>
-    <hyperlink ref="J12" r:id="rId25" xr:uid="{5A506C84-4FD5-4C15-9819-9ADA9D37E63C}"/>
-    <hyperlink ref="J18" r:id="rId26" xr:uid="{66DCDBD3-0A17-4F25-A19C-055A4209733C}"/>
-    <hyperlink ref="J26" r:id="rId27" xr:uid="{DEB2DF39-759A-4E16-A9AB-E96ECF63A544}"/>
+    <hyperlink ref="J19" r:id="rId1" xr:uid="{5EB9FB3D-22AD-47DC-B125-539430A9CC29}"/>
+    <hyperlink ref="J15" r:id="rId2" xr:uid="{53BAB52E-738A-40FD-AE11-30F4B5C07642}"/>
+    <hyperlink ref="J20" r:id="rId3" xr:uid="{D254588B-7BF2-4663-B764-31CEE1702B72}"/>
+    <hyperlink ref="J21" r:id="rId4" xr:uid="{97844978-768D-4AF2-9FC1-EA6B6AEA91A7}"/>
+    <hyperlink ref="J2" r:id="rId5" xr:uid="{A783C18C-5336-47D4-B91E-5A0D50EFD847}"/>
+    <hyperlink ref="J23" r:id="rId6" xr:uid="{DA2D5093-8FE6-45A4-BA10-918A48B82B08}"/>
+    <hyperlink ref="J22" r:id="rId7" xr:uid="{F70812B2-9C02-459F-B38C-705355029FE7}"/>
+    <hyperlink ref="J24" r:id="rId8" xr:uid="{3F47DA3C-1E53-444A-8898-B9EA85FBD647}"/>
+    <hyperlink ref="J25" r:id="rId9" xr:uid="{13709938-D199-4718-8973-2310F69E82EA}"/>
+    <hyperlink ref="A35" r:id="rId10" xr:uid="{9308F7BC-A83E-47C6-82E4-B9074942D108}"/>
+    <hyperlink ref="J6" r:id="rId11" xr:uid="{97C57276-2433-4923-8B77-CF1D09F8B548}"/>
+    <hyperlink ref="J7" r:id="rId12" xr:uid="{FC24FC01-0AA7-4D5B-BEA8-DAA6380AC073}"/>
+    <hyperlink ref="J8" r:id="rId13" xr:uid="{384DB0BE-F1AE-4448-80D7-0387BA330343}"/>
+    <hyperlink ref="J4" r:id="rId14" xr:uid="{E60A837F-D0CD-4E15-8F80-70CC3A0226A6}"/>
+    <hyperlink ref="J5" r:id="rId15" xr:uid="{4A829B53-4217-4F26-89B4-F106E6B544CD}"/>
+    <hyperlink ref="J14" r:id="rId16" xr:uid="{305F8F85-0874-4D1F-9E8A-6D0403800691}"/>
+    <hyperlink ref="K13" r:id="rId17" xr:uid="{E0DF6966-BBD6-4D0C-B6F6-D79BAA6169DB}"/>
+    <hyperlink ref="J9" r:id="rId18" xr:uid="{9DC153CF-6A36-4F67-AFC5-22DD9E35702B}"/>
+    <hyperlink ref="J10" r:id="rId19" xr:uid="{AEFCF35C-6C14-479F-9C9D-A9454FACE026}"/>
+    <hyperlink ref="J13" r:id="rId20" xr:uid="{AA52E67F-B095-4E7F-9662-B6B8C8564EF9}"/>
+    <hyperlink ref="J17" r:id="rId21" xr:uid="{4A1380DF-B3F7-4272-8054-E7C4BBA79028}"/>
+    <hyperlink ref="J16" r:id="rId22" xr:uid="{8C9B92D8-2E44-4B6A-B72A-0A081445CCF4}"/>
+    <hyperlink ref="J11" r:id="rId23" xr:uid="{3FB67847-D385-4555-A810-A1F070CC4594}"/>
+    <hyperlink ref="J12" r:id="rId24" xr:uid="{5A506C84-4FD5-4C15-9819-9ADA9D37E63C}"/>
+    <hyperlink ref="J18" r:id="rId25" xr:uid="{66DCDBD3-0A17-4F25-A19C-055A4209733C}"/>
+    <hyperlink ref="J26" r:id="rId26" xr:uid="{DEB2DF39-759A-4E16-A9AB-E96ECF63A544}"/>
+    <hyperlink ref="J3" r:id="rId27" xr:uid="{A2771846-5465-4023-A9E5-D8F1D4061B69}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId28"/>

</xml_diff>

<commit_message>
Added latest orders to Expense Report and updated Bill of Materials with M4 screws and nuts for new Tower modification
</commit_message>
<xml_diff>
--- a/Ordered Parts/Bill of Materials.xlsx
+++ b/Ordered Parts/Bill of Materials.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803EFA5C-5C1C-488F-9ADA-FDBA02B04063}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8077AA-67EC-4A3D-A34B-2BE90F517696}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11508" windowHeight="8796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11505" windowHeight="8790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="154">
   <si>
     <t>Part</t>
   </si>
@@ -229,9 +229,6 @@
     <t>PCB Fabrication</t>
   </si>
   <si>
-    <t>Alternate PCB Assembly Quote</t>
-  </si>
-  <si>
     <t>M3 Screws</t>
   </si>
   <si>
@@ -274,9 +271,6 @@
     <t>A12092200UX0087</t>
   </si>
   <si>
-    <t xml:space="preserve"> A13092700UX0955</t>
-  </si>
-  <si>
     <t>700724341402</t>
   </si>
   <si>
@@ -452,6 +446,42 @@
   </si>
   <si>
     <t>B00DKSI0S8</t>
+  </si>
+  <si>
+    <t>M4 Screws</t>
+  </si>
+  <si>
+    <t>M4 Nuts</t>
+  </si>
+  <si>
+    <t>Small Parts</t>
+  </si>
+  <si>
+    <t>B00F32EDI0</t>
+  </si>
+  <si>
+    <t>FSCM440JISSZ</t>
+  </si>
+  <si>
+    <t>Steel Machine Screw, Zinc Plated, M4, 40 mm Length</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B00F32EDI0/ref=oh_aui_detailpage_o00_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>A13092700UX0955</t>
+  </si>
+  <si>
+    <t>A15052500UX0288</t>
+  </si>
+  <si>
+    <t>B0143GL55A</t>
+  </si>
+  <si>
+    <t>Metric M4 Hex Nut 304 Stainless Steel Fastener 100pcs</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B0143GL55A/ref=oh_aui_detailpage_o00_s00?ie=UTF8&amp;psc=1</t>
   </si>
 </sst>
 </file>
@@ -816,26 +846,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="5"/>
-    <col min="8" max="8" width="9.21875" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="51.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="5"/>
+    <col min="8" max="8" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -867,7 +897,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -884,7 +914,7 @@
         <v>13</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G2" s="5">
         <f>18.95/50</f>
@@ -901,7 +931,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -909,16 +939,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G3" s="5">
         <v>9.99</v>
@@ -928,30 +958,30 @@
         <v>9.99</v>
       </c>
       <c r="I3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G4" s="5">
         <f>6.97/100</f>
@@ -962,30 +992,30 @@
         <v>0.1394</v>
       </c>
       <c r="I4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G5" s="5">
         <f>8.62/200</f>
@@ -996,57 +1026,57 @@
         <v>8.6199999999999999E-2</v>
       </c>
       <c r="I5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" t="s">
         <v>75</v>
-      </c>
-      <c r="D6" t="s">
-        <v>76</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G6" s="5">
         <v>0.10340000000000001</v>
       </c>
       <c r="H6" s="5">
-        <f t="shared" ref="H6:H8" si="1">B6*G6</f>
+        <f t="shared" ref="H6:H10" si="1">B6*G6</f>
         <v>0.41360000000000002</v>
       </c>
       <c r="I6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -1062,30 +1092,30 @@
         <v>0.55759999999999998</v>
       </c>
       <c r="I7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>84</v>
+        <v>149</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G8" s="5">
         <v>4.6100000000000002E-2</v>
@@ -1095,253 +1125,255 @@
         <v>0.18440000000000001</v>
       </c>
       <c r="I8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>142</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>111</v>
+        <v>144</v>
+      </c>
+      <c r="D9" t="s">
+        <v>146</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>112</v>
+      <c r="F9" t="s">
+        <v>145</v>
       </c>
       <c r="G9" s="5">
+        <f>4.08/25</f>
+        <v>0.16320000000000001</v>
+      </c>
+      <c r="H9" s="5">
+        <f t="shared" si="1"/>
+        <v>0.16320000000000001</v>
+      </c>
+      <c r="I9" t="s">
+        <v>147</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" t="s">
+        <v>150</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="G10" s="5">
+        <f>7.25/100</f>
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="H10" s="5">
+        <f t="shared" si="1"/>
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="I10" t="s">
+        <v>152</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G11" s="5">
         <f>11.86/3</f>
         <v>3.9533333333333331</v>
       </c>
-      <c r="H9" s="5">
-        <f>B9*G9</f>
+      <c r="H11" s="5">
+        <f>B11*G11</f>
         <v>3.9533333333333331</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I11" t="s">
+        <v>111</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="G12" s="5">
+        <v>2.99</v>
+      </c>
+      <c r="H12" s="5">
+        <f>B12*G12</f>
+        <v>2.99</v>
+      </c>
+      <c r="I12" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="J12" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" s="3" t="s">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="E10" t="s">
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>125</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E13" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="G10" s="5">
-        <v>2.99</v>
-      </c>
-      <c r="H10" s="5">
-        <f>B10*G10</f>
-        <v>2.99</v>
-      </c>
-      <c r="I10" t="s">
-        <v>107</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>127</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="G11" s="9">
+      <c r="F13" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G13" s="9">
         <f>11.54/50</f>
         <v>0.23079999999999998</v>
       </c>
-      <c r="H11" s="5">
-        <f>B11*G11</f>
+      <c r="H13" s="5">
+        <f>B13*G13</f>
         <v>0.6923999999999999</v>
       </c>
-      <c r="I11" t="s">
-        <v>126</v>
-      </c>
-      <c r="J11" s="10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="I13" t="s">
+        <v>124</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
         <v>129</v>
       </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" t="s">
-        <v>130</v>
-      </c>
-      <c r="E12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" t="s">
-        <v>131</v>
-      </c>
-      <c r="G12" s="5">
+      <c r="G14" s="5">
         <f>11.6/100</f>
         <v>0.11599999999999999</v>
       </c>
-      <c r="H12" s="5">
-        <f>B12*G12</f>
+      <c r="H14" s="5">
+        <f>B14*G14</f>
         <v>0.23199999999999998</v>
       </c>
-      <c r="I12" t="s">
-        <v>132</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="I14" t="s">
+        <v>130</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="B13">
+      <c r="B15">
         <v>1</v>
       </c>
-      <c r="C13" t="s">
-        <v>102</v>
-      </c>
-      <c r="D13" t="s">
-        <v>101</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="C15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15" t="s">
         <v>8</v>
       </c>
-      <c r="F13" t="s">
-        <v>101</v>
-      </c>
-      <c r="G13" s="5">
+      <c r="F15" t="s">
+        <v>99</v>
+      </c>
+      <c r="G15" s="5">
         <f>((11.56*56)+(11.79*44))/100</f>
         <v>11.661199999999999</v>
       </c>
-      <c r="H13" s="5">
-        <f>B13*G13</f>
-        <v>11.661199999999999</v>
-      </c>
-      <c r="I13" t="s">
-        <v>110</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" t="s">
-        <v>100</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" t="s">
-        <v>100</v>
-      </c>
-      <c r="G14" s="5">
-        <v>9.73</v>
-      </c>
-      <c r="H14" s="5">
-        <f t="shared" ref="H14:H26" si="2">B14*G14</f>
-        <v>9.73</v>
-      </c>
-      <c r="I14" t="s">
-        <v>99</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" t="s">
-        <v>29</v>
-      </c>
-      <c r="G15" s="5">
-        <v>0.01</v>
-      </c>
       <c r="H15" s="5">
         <f>B15*G15</f>
-        <v>0.01</v>
+        <v>11.661199999999999</v>
       </c>
       <c r="I15" t="s">
-        <v>28</v>
+        <v>108</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>119</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1349,428 +1381,490 @@
       <c r="C16" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>118</v>
+      <c r="D16" t="s">
+        <v>98</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="G16" s="9">
+      <c r="F16" t="s">
+        <v>98</v>
+      </c>
+      <c r="G16" s="5">
+        <v>9.73</v>
+      </c>
+      <c r="H16" s="5">
+        <f t="shared" ref="H16:H28" si="2">B16*G16</f>
+        <v>9.73</v>
+      </c>
+      <c r="I16" t="s">
+        <v>97</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="H17" s="5">
+        <f>B17*G17</f>
+        <v>0.01</v>
+      </c>
+      <c r="I17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G18" s="9">
         <f>4.8/49</f>
         <v>9.7959183673469383E-2</v>
       </c>
-      <c r="H16" s="5">
-        <f t="shared" ref="H16:H17" si="3">B16*G16</f>
+      <c r="H18" s="5">
+        <f t="shared" ref="H18:H19" si="3">B18*G18</f>
         <v>9.7959183673469383E-2</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I18" t="s">
+        <v>120</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="J16" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>120</v>
-      </c>
-      <c r="B17">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>118</v>
+      </c>
+      <c r="B19">
         <v>1</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C19" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="D19" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E19" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="G17" s="9">
+      <c r="F19" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G19" s="9">
         <f>4.8/49</f>
         <v>9.7959183673469383E-2</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H19" s="5">
         <f t="shared" si="3"/>
         <v>9.7959183673469383E-2</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I19" t="s">
+        <v>119</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
+    </row>
+    <row r="20" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B20" s="11">
         <v>1</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="E18" s="11" t="s">
+      <c r="C20" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="G18" s="13">
+      <c r="F20" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="G20" s="13">
         <v>0.58450000000000002</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H20" s="13">
         <f t="shared" si="2"/>
         <v>0.58450000000000002</v>
       </c>
-      <c r="I18" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="J18" s="10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="I20" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>21</v>
       </c>
-      <c r="B19">
+      <c r="B21">
         <v>1</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C21" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E21" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G21" s="5">
         <v>0.90280000000000005</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H21" s="5">
         <f t="shared" si="2"/>
         <v>0.90280000000000005</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I21" t="s">
         <v>24</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="J21" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>32</v>
       </c>
-      <c r="B20">
+      <c r="B22">
         <v>1</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C22" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E22" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G22" s="5">
         <v>0.53400000000000003</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H22" s="5">
         <f t="shared" si="2"/>
         <v>0.53400000000000003</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I22" t="s">
         <v>36</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="J22" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>33</v>
       </c>
-      <c r="B21">
+      <c r="B23">
         <v>1</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C23" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E23" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F23" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G23" s="5">
         <v>0.63229999999999997</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H23" s="5">
         <f t="shared" si="2"/>
         <v>0.63229999999999997</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I23" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="J23" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>47</v>
       </c>
-      <c r="B22">
+      <c r="B24">
         <v>10</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C24" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E24" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F24" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G24" s="5">
         <v>3.0300000000000001E-2</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H24" s="5">
         <f t="shared" si="2"/>
         <v>0.30299999999999999</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I24" t="s">
         <v>50</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="J24" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>52</v>
       </c>
-      <c r="B23">
+      <c r="B25">
         <v>2</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C25" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E25" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G25" s="5">
         <v>3.8100000000000002E-2</v>
       </c>
-      <c r="H23" s="5">
+      <c r="H25" s="5">
         <f t="shared" si="2"/>
         <v>7.6200000000000004E-2</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I25" t="s">
         <v>54</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="J25" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>56</v>
       </c>
-      <c r="B24">
+      <c r="B26">
         <v>1</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C26" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E26" t="s">
         <v>19</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G26" s="5">
         <v>7.5899999999999995E-2</v>
       </c>
-      <c r="H24" s="5">
+      <c r="H26" s="5">
         <f t="shared" si="2"/>
         <v>7.5899999999999995E-2</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I26" t="s">
         <v>58</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="J26" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>60</v>
       </c>
-      <c r="B25">
+      <c r="B27">
         <v>2</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C27" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E27" t="s">
         <v>19</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F27" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G27" s="5">
         <v>6.3799999999999996E-2</v>
       </c>
-      <c r="H25" s="5">
+      <c r="H27" s="5">
         <f t="shared" si="2"/>
         <v>0.12759999999999999</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I27" t="s">
         <v>62</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="J27" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>68</v>
       </c>
-      <c r="B26">
+      <c r="B28">
         <v>1</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C28" t="s">
         <v>64</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E28" t="s">
         <v>64</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F28" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G28" s="5">
         <v>0.3871</v>
       </c>
-      <c r="H26" s="5">
+      <c r="H28" s="5">
         <f t="shared" si="2"/>
         <v>0.3871</v>
       </c>
-      <c r="I26" t="s">
-        <v>138</v>
-      </c>
-      <c r="J26" s="2" t="s">
+      <c r="I28" t="s">
+        <v>136</v>
+      </c>
+      <c r="J28" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G27" s="4" t="s">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G29" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H27" s="5">
-        <f>SUM(H2:H26)</f>
-        <v>45.217451700680265</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+      <c r="H29" s="5">
+        <f>SUM(H2:H28)</f>
+        <v>45.453151700680259</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G28" s="4"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J30" s="2"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J31" s="2"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>69</v>
-      </c>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J33" s="2"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J19" r:id="rId1" xr:uid="{5EB9FB3D-22AD-47DC-B125-539430A9CC29}"/>
-    <hyperlink ref="J15" r:id="rId2" xr:uid="{53BAB52E-738A-40FD-AE11-30F4B5C07642}"/>
-    <hyperlink ref="J20" r:id="rId3" xr:uid="{D254588B-7BF2-4663-B764-31CEE1702B72}"/>
-    <hyperlink ref="J21" r:id="rId4" xr:uid="{97844978-768D-4AF2-9FC1-EA6B6AEA91A7}"/>
+    <hyperlink ref="J21" r:id="rId1" xr:uid="{5EB9FB3D-22AD-47DC-B125-539430A9CC29}"/>
+    <hyperlink ref="J17" r:id="rId2" xr:uid="{53BAB52E-738A-40FD-AE11-30F4B5C07642}"/>
+    <hyperlink ref="J22" r:id="rId3" xr:uid="{D254588B-7BF2-4663-B764-31CEE1702B72}"/>
+    <hyperlink ref="J23" r:id="rId4" xr:uid="{97844978-768D-4AF2-9FC1-EA6B6AEA91A7}"/>
     <hyperlink ref="J2" r:id="rId5" xr:uid="{A783C18C-5336-47D4-B91E-5A0D50EFD847}"/>
-    <hyperlink ref="J23" r:id="rId6" xr:uid="{DA2D5093-8FE6-45A4-BA10-918A48B82B08}"/>
-    <hyperlink ref="J22" r:id="rId7" xr:uid="{F70812B2-9C02-459F-B38C-705355029FE7}"/>
-    <hyperlink ref="J24" r:id="rId8" xr:uid="{3F47DA3C-1E53-444A-8898-B9EA85FBD647}"/>
-    <hyperlink ref="J25" r:id="rId9" xr:uid="{13709938-D199-4718-8973-2310F69E82EA}"/>
-    <hyperlink ref="A35" r:id="rId10" xr:uid="{9308F7BC-A83E-47C6-82E4-B9074942D108}"/>
-    <hyperlink ref="J6" r:id="rId11" xr:uid="{97C57276-2433-4923-8B77-CF1D09F8B548}"/>
-    <hyperlink ref="J7" r:id="rId12" xr:uid="{FC24FC01-0AA7-4D5B-BEA8-DAA6380AC073}"/>
-    <hyperlink ref="J8" r:id="rId13" xr:uid="{384DB0BE-F1AE-4448-80D7-0387BA330343}"/>
-    <hyperlink ref="J4" r:id="rId14" xr:uid="{E60A837F-D0CD-4E15-8F80-70CC3A0226A6}"/>
-    <hyperlink ref="J5" r:id="rId15" xr:uid="{4A829B53-4217-4F26-89B4-F106E6B544CD}"/>
-    <hyperlink ref="J14" r:id="rId16" xr:uid="{305F8F85-0874-4D1F-9E8A-6D0403800691}"/>
-    <hyperlink ref="K13" r:id="rId17" xr:uid="{E0DF6966-BBD6-4D0C-B6F6-D79BAA6169DB}"/>
-    <hyperlink ref="J9" r:id="rId18" xr:uid="{9DC153CF-6A36-4F67-AFC5-22DD9E35702B}"/>
-    <hyperlink ref="J10" r:id="rId19" xr:uid="{AEFCF35C-6C14-479F-9C9D-A9454FACE026}"/>
-    <hyperlink ref="J13" r:id="rId20" xr:uid="{AA52E67F-B095-4E7F-9662-B6B8C8564EF9}"/>
-    <hyperlink ref="J17" r:id="rId21" xr:uid="{4A1380DF-B3F7-4272-8054-E7C4BBA79028}"/>
-    <hyperlink ref="J16" r:id="rId22" xr:uid="{8C9B92D8-2E44-4B6A-B72A-0A081445CCF4}"/>
-    <hyperlink ref="J11" r:id="rId23" xr:uid="{3FB67847-D385-4555-A810-A1F070CC4594}"/>
-    <hyperlink ref="J12" r:id="rId24" xr:uid="{5A506C84-4FD5-4C15-9819-9ADA9D37E63C}"/>
-    <hyperlink ref="J18" r:id="rId25" xr:uid="{66DCDBD3-0A17-4F25-A19C-055A4209733C}"/>
-    <hyperlink ref="J26" r:id="rId26" xr:uid="{DEB2DF39-759A-4E16-A9AB-E96ECF63A544}"/>
-    <hyperlink ref="J3" r:id="rId27" xr:uid="{A2771846-5465-4023-A9E5-D8F1D4061B69}"/>
+    <hyperlink ref="J25" r:id="rId6" xr:uid="{DA2D5093-8FE6-45A4-BA10-918A48B82B08}"/>
+    <hyperlink ref="J24" r:id="rId7" xr:uid="{F70812B2-9C02-459F-B38C-705355029FE7}"/>
+    <hyperlink ref="J26" r:id="rId8" xr:uid="{3F47DA3C-1E53-444A-8898-B9EA85FBD647}"/>
+    <hyperlink ref="J27" r:id="rId9" xr:uid="{13709938-D199-4718-8973-2310F69E82EA}"/>
+    <hyperlink ref="J6" r:id="rId10" xr:uid="{97C57276-2433-4923-8B77-CF1D09F8B548}"/>
+    <hyperlink ref="J7" r:id="rId11" xr:uid="{FC24FC01-0AA7-4D5B-BEA8-DAA6380AC073}"/>
+    <hyperlink ref="J8" r:id="rId12" xr:uid="{384DB0BE-F1AE-4448-80D7-0387BA330343}"/>
+    <hyperlink ref="J4" r:id="rId13" xr:uid="{E60A837F-D0CD-4E15-8F80-70CC3A0226A6}"/>
+    <hyperlink ref="J5" r:id="rId14" xr:uid="{4A829B53-4217-4F26-89B4-F106E6B544CD}"/>
+    <hyperlink ref="J16" r:id="rId15" xr:uid="{305F8F85-0874-4D1F-9E8A-6D0403800691}"/>
+    <hyperlink ref="K15" r:id="rId16" xr:uid="{E0DF6966-BBD6-4D0C-B6F6-D79BAA6169DB}"/>
+    <hyperlink ref="J11" r:id="rId17" xr:uid="{9DC153CF-6A36-4F67-AFC5-22DD9E35702B}"/>
+    <hyperlink ref="J12" r:id="rId18" xr:uid="{AEFCF35C-6C14-479F-9C9D-A9454FACE026}"/>
+    <hyperlink ref="J15" r:id="rId19" xr:uid="{AA52E67F-B095-4E7F-9662-B6B8C8564EF9}"/>
+    <hyperlink ref="J19" r:id="rId20" xr:uid="{4A1380DF-B3F7-4272-8054-E7C4BBA79028}"/>
+    <hyperlink ref="J18" r:id="rId21" xr:uid="{8C9B92D8-2E44-4B6A-B72A-0A081445CCF4}"/>
+    <hyperlink ref="J13" r:id="rId22" xr:uid="{3FB67847-D385-4555-A810-A1F070CC4594}"/>
+    <hyperlink ref="J14" r:id="rId23" xr:uid="{5A506C84-4FD5-4C15-9819-9ADA9D37E63C}"/>
+    <hyperlink ref="J20" r:id="rId24" xr:uid="{66DCDBD3-0A17-4F25-A19C-055A4209733C}"/>
+    <hyperlink ref="J28" r:id="rId25" xr:uid="{DEB2DF39-759A-4E16-A9AB-E96ECF63A544}"/>
+    <hyperlink ref="J3" r:id="rId26" xr:uid="{A2771846-5465-4023-A9E5-D8F1D4061B69}"/>
+    <hyperlink ref="J9" r:id="rId27" xr:uid="{B027D582-DB2E-46D9-8854-474EB0EBDFB0}"/>
+    <hyperlink ref="J10" r:id="rId28" xr:uid="{F077A7B0-1644-4316-9D46-032403F3533F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId28"/>
+  <pageSetup orientation="portrait" r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added most recent Amazon Order for heatshrink tubing to expense report
</commit_message>
<xml_diff>
--- a/Ordered Parts/Bill of Materials.xlsx
+++ b/Ordered Parts/Bill of Materials.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8077AA-67EC-4A3D-A34B-2BE90F517696}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38A4027-F7EA-451F-9A03-F609840C3808}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11505" windowHeight="8790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="155">
   <si>
     <t>Part</t>
   </si>
@@ -337,12 +337,6 @@
     <t>Programming Cable</t>
   </si>
   <si>
-    <t>StarTech 1-Feet Mini USB 2.0 Cable - A to Mini B</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/gp/product/B002L5U7N2/ref=ox_sc_act_title_7?smid=ATVPDKIKX0DER&amp;psc=1</t>
-  </si>
-  <si>
     <t>https://hobbyking.com/en_us/m1306l-brushless-motor-for-rc-model-aircraft-ccw.html</t>
   </si>
   <si>
@@ -358,12 +352,6 @@
     <t>Arduino Nano V3.0, Elegoo Nano ATmega328P</t>
   </si>
   <si>
-    <t>USB2HABM1</t>
-  </si>
-  <si>
-    <t>B002L5U7N2</t>
-  </si>
-  <si>
     <t>Bullet Plugs</t>
   </si>
   <si>
@@ -482,6 +470,21 @@
   </si>
   <si>
     <t>https://www.amazon.com/gp/product/B0143GL55A/ref=oh_aui_detailpage_o00_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>AmazonBasics</t>
+  </si>
+  <si>
+    <t>B0718XZKWH</t>
+  </si>
+  <si>
+    <t>3S44_24</t>
+  </si>
+  <si>
+    <t>USB 2.0 Cable - A-Male to Mini-B, 3 Feet (0.9 Meters)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B0718XZKWH/ref=oh_aui_detailpage_o03_s00?ie=UTF8&amp;psc=1</t>
   </si>
 </sst>
 </file>
@@ -848,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,16 +942,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G3" s="5">
         <v>9.99</v>
@@ -958,10 +961,10 @@
         <v>9.99</v>
       </c>
       <c r="I3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1109,7 +1112,7 @@
         <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
@@ -1133,22 +1136,22 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G9" s="5">
         <f>4.08/25</f>
@@ -1159,15 +1162,15 @@
         <v>0.16320000000000001</v>
       </c>
       <c r="I9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1176,13 +1179,13 @@
         <v>73</v>
       </c>
       <c r="D10" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G10" s="5">
         <f>7.25/100</f>
@@ -1193,10 +1196,10 @@
         <v>7.2499999999999995E-2</v>
       </c>
       <c r="I10" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1210,13 +1213,13 @@
         <v>102</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G11" s="5">
         <f>11.86/3</f>
@@ -1227,7 +1230,7 @@
         <v>3.9533333333333331</v>
       </c>
       <c r="I11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>103</v>
@@ -1241,49 +1244,50 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>150</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>112</v>
+        <v>152</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>113</v>
+        <v>151</v>
       </c>
       <c r="G12" s="5">
-        <v>2.99</v>
+        <f>47.99/24</f>
+        <v>1.9995833333333335</v>
       </c>
       <c r="H12" s="5">
         <f>B12*G12</f>
-        <v>2.99</v>
+        <v>1.9995833333333335</v>
       </c>
       <c r="I12" t="s">
-        <v>105</v>
+        <v>153</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>106</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G13" s="9">
         <f>11.54/50</f>
@@ -1294,15 +1298,15 @@
         <v>0.6923999999999999</v>
       </c>
       <c r="I13" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -1311,13 +1315,13 @@
         <v>73</v>
       </c>
       <c r="D14" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E14" t="s">
         <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G14" s="5">
         <f>11.6/100</f>
@@ -1328,10 +1332,10 @@
         <v>0.23199999999999998</v>
       </c>
       <c r="I14" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1362,10 +1366,10 @@
         <v>11.661199999999999</v>
       </c>
       <c r="I15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>101</v>
@@ -1439,7 +1443,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1448,13 +1452,13 @@
         <v>16</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E18" t="s">
         <v>8</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G18" s="9">
         <f>4.8/49</f>
@@ -1465,15 +1469,15 @@
         <v>9.7959183673469383E-2</v>
       </c>
       <c r="I18" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1482,13 +1486,13 @@
         <v>16</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G19" s="9">
         <f>4.8/49</f>
@@ -1499,10 +1503,10 @@
         <v>9.7959183673469383E-2</v>
       </c>
       <c r="I19" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -1513,16 +1517,16 @@
         <v>1</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>19</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G20" s="13">
         <v>0.58450000000000002</v>
@@ -1532,10 +1536,10 @@
         <v>0.58450000000000002</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1796,7 +1800,7 @@
         <v>0.3871</v>
       </c>
       <c r="I28" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>67</v>
@@ -1808,7 +1812,7 @@
       </c>
       <c r="H29" s="5">
         <f>SUM(H2:H28)</f>
-        <v>45.453151700680259</v>
+        <v>44.462735034013583</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1852,17 +1856,17 @@
     <hyperlink ref="J16" r:id="rId15" xr:uid="{305F8F85-0874-4D1F-9E8A-6D0403800691}"/>
     <hyperlink ref="K15" r:id="rId16" xr:uid="{E0DF6966-BBD6-4D0C-B6F6-D79BAA6169DB}"/>
     <hyperlink ref="J11" r:id="rId17" xr:uid="{9DC153CF-6A36-4F67-AFC5-22DD9E35702B}"/>
-    <hyperlink ref="J12" r:id="rId18" xr:uid="{AEFCF35C-6C14-479F-9C9D-A9454FACE026}"/>
-    <hyperlink ref="J15" r:id="rId19" xr:uid="{AA52E67F-B095-4E7F-9662-B6B8C8564EF9}"/>
-    <hyperlink ref="J19" r:id="rId20" xr:uid="{4A1380DF-B3F7-4272-8054-E7C4BBA79028}"/>
-    <hyperlink ref="J18" r:id="rId21" xr:uid="{8C9B92D8-2E44-4B6A-B72A-0A081445CCF4}"/>
-    <hyperlink ref="J13" r:id="rId22" xr:uid="{3FB67847-D385-4555-A810-A1F070CC4594}"/>
-    <hyperlink ref="J14" r:id="rId23" xr:uid="{5A506C84-4FD5-4C15-9819-9ADA9D37E63C}"/>
-    <hyperlink ref="J20" r:id="rId24" xr:uid="{66DCDBD3-0A17-4F25-A19C-055A4209733C}"/>
-    <hyperlink ref="J28" r:id="rId25" xr:uid="{DEB2DF39-759A-4E16-A9AB-E96ECF63A544}"/>
-    <hyperlink ref="J3" r:id="rId26" xr:uid="{A2771846-5465-4023-A9E5-D8F1D4061B69}"/>
-    <hyperlink ref="J9" r:id="rId27" xr:uid="{B027D582-DB2E-46D9-8854-474EB0EBDFB0}"/>
-    <hyperlink ref="J10" r:id="rId28" xr:uid="{F077A7B0-1644-4316-9D46-032403F3533F}"/>
+    <hyperlink ref="J15" r:id="rId18" xr:uid="{AA52E67F-B095-4E7F-9662-B6B8C8564EF9}"/>
+    <hyperlink ref="J19" r:id="rId19" xr:uid="{4A1380DF-B3F7-4272-8054-E7C4BBA79028}"/>
+    <hyperlink ref="J18" r:id="rId20" xr:uid="{8C9B92D8-2E44-4B6A-B72A-0A081445CCF4}"/>
+    <hyperlink ref="J13" r:id="rId21" xr:uid="{3FB67847-D385-4555-A810-A1F070CC4594}"/>
+    <hyperlink ref="J14" r:id="rId22" xr:uid="{5A506C84-4FD5-4C15-9819-9ADA9D37E63C}"/>
+    <hyperlink ref="J20" r:id="rId23" xr:uid="{66DCDBD3-0A17-4F25-A19C-055A4209733C}"/>
+    <hyperlink ref="J28" r:id="rId24" xr:uid="{DEB2DF39-759A-4E16-A9AB-E96ECF63A544}"/>
+    <hyperlink ref="J3" r:id="rId25" xr:uid="{A2771846-5465-4023-A9E5-D8F1D4061B69}"/>
+    <hyperlink ref="J9" r:id="rId26" xr:uid="{B027D582-DB2E-46D9-8854-474EB0EBDFB0}"/>
+    <hyperlink ref="J10" r:id="rId27" xr:uid="{F077A7B0-1644-4316-9D46-032403F3533F}"/>
+    <hyperlink ref="J12" r:id="rId28" xr:uid="{06C67DAE-C4AF-4036-B24C-1BF0591900B9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId29"/>

</xml_diff>

<commit_message>
Added heat shrink tubing to Bill of Materials
</commit_message>
<xml_diff>
--- a/Ordered Parts/Bill of Materials.xlsx
+++ b/Ordered Parts/Bill of Materials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38A4027-F7EA-451F-9A03-F609840C3808}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4BD16EB-5CE1-4F9E-A925-752CD5B0CBBC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11505" windowHeight="8790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11508" windowHeight="8790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="166">
   <si>
     <t>Part</t>
   </si>
@@ -100,9 +100,6 @@
     <t>https://www.arrow.com/en/products/sv03a103aea01r00/murata-manufacturing</t>
   </si>
   <si>
-    <t>Heat Shrink</t>
-  </si>
-  <si>
     <t>PLA</t>
   </si>
   <si>
@@ -485,6 +482,42 @@
   </si>
   <si>
     <t>https://www.amazon.com/gp/product/B0718XZKWH/ref=oh_aui_detailpage_o03_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>2:1 Heat Shrink Tubing</t>
+  </si>
+  <si>
+    <t>3:1 Heat Shrink Tubing</t>
+  </si>
+  <si>
+    <t>Innhom</t>
+  </si>
+  <si>
+    <t>Ginsco</t>
+  </si>
+  <si>
+    <t>B075WR9FVL</t>
+  </si>
+  <si>
+    <t>HS-532B</t>
+  </si>
+  <si>
+    <t>A270</t>
+  </si>
+  <si>
+    <t>610731355845</t>
+  </si>
+  <si>
+    <t>270Pcs 3:1 Dual Wall Adhesive Lined Heat Shrink Tubing Kit</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B073R69KNB/ref=oh_aui_detailpage_o01_s01?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>532pcs 2:1 Heat Shrink Tubing Insulation Protection Kit</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B075WR9FVL/ref=oh_aui_detailpage_o01_s00?ie=UTF8&amp;psc=1</t>
   </si>
 </sst>
 </file>
@@ -849,26 +882,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="5"/>
-    <col min="8" max="8" width="9.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="51.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.83984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.15625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83984375" style="5"/>
+    <col min="8" max="8" width="9.15625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="51.15625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -900,7 +933,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -908,16 +941,16 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G2" s="5">
         <f>18.95/50</f>
@@ -928,13 +961,13 @@
         <v>0.75800000000000001</v>
       </c>
       <c r="I2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -942,16 +975,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G3" s="5">
         <v>9.99</v>
@@ -961,30 +994,30 @@
         <v>9.99</v>
       </c>
       <c r="I3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G4" s="5">
         <f>6.97/100</f>
@@ -995,30 +1028,30 @@
         <v>0.1394</v>
       </c>
       <c r="I4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G5" s="5">
         <f>8.62/200</f>
@@ -1029,30 +1062,30 @@
         <v>8.6199999999999999E-2</v>
       </c>
       <c r="I5" t="s">
+        <v>93</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" t="s">
         <v>74</v>
-      </c>
-      <c r="D6" t="s">
-        <v>75</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G6" s="5">
         <v>0.10340000000000001</v>
@@ -1062,24 +1095,24 @@
         <v>0.41360000000000002</v>
       </c>
       <c r="I6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -1095,30 +1128,30 @@
         <v>0.55759999999999998</v>
       </c>
       <c r="I7" t="s">
+        <v>79</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G8" s="5">
         <v>4.6100000000000002E-2</v>
@@ -1128,30 +1161,30 @@
         <v>0.18440000000000001</v>
       </c>
       <c r="I8" t="s">
+        <v>83</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G9" s="5">
         <f>4.08/25</f>
@@ -1162,30 +1195,30 @@
         <v>0.16320000000000001</v>
       </c>
       <c r="I9" t="s">
+        <v>142</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G10" s="5">
         <f>7.25/100</f>
@@ -1196,13 +1229,13 @@
         <v>7.2499999999999995E-2</v>
       </c>
       <c r="I10" t="s">
+        <v>147</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1210,16 +1243,16 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G11" s="5">
         <f>11.86/3</f>
@@ -1230,30 +1263,30 @@
         <v>3.9533333333333331</v>
       </c>
       <c r="I11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J11" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>104</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G12" s="5">
         <f>47.99/24</f>
@@ -1264,30 +1297,30 @@
         <v>1.9995833333333335</v>
       </c>
       <c r="I12" t="s">
+        <v>152</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
       <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>122</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G13" s="9">
         <f>11.54/50</f>
@@ -1298,30 +1331,30 @@
         <v>0.6923999999999999</v>
       </c>
       <c r="I13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E14" t="s">
         <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G14" s="5">
         <f>11.6/100</f>
@@ -1332,118 +1365,120 @@
         <v>0.23199999999999998</v>
       </c>
       <c r="I14" t="s">
+        <v>125</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>154</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>100</v>
+        <v>156</v>
       </c>
       <c r="D15" t="s">
+        <v>159</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" t="s">
+        <v>158</v>
+      </c>
+      <c r="G15" s="5">
+        <f>(2*7.99)/100</f>
+        <v>0.1598</v>
+      </c>
+      <c r="H15" s="5">
+        <f>B15*G15</f>
+        <v>0.1598</v>
+      </c>
+      <c r="I15" t="s">
+        <v>164</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>155</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D16" t="s">
+        <v>160</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="G16" s="5">
+        <f>(9.99+8.99)/100</f>
+        <v>0.1898</v>
+      </c>
+      <c r="H16" s="5">
+        <f>B16*G16</f>
+        <v>0.1898</v>
+      </c>
+      <c r="I16" t="s">
+        <v>162</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
         <v>99</v>
       </c>
-      <c r="E15" t="s">
+      <c r="D17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" t="s">
         <v>8</v>
       </c>
-      <c r="F15" t="s">
-        <v>99</v>
-      </c>
-      <c r="G15" s="5">
+      <c r="F17" t="s">
+        <v>98</v>
+      </c>
+      <c r="G17" s="5">
         <f>((11.56*56)+(11.79*44))/100</f>
         <v>11.661199999999999</v>
       </c>
-      <c r="H15" s="5">
-        <f>B15*G15</f>
-        <v>11.661199999999999</v>
-      </c>
-      <c r="I15" t="s">
-        <v>106</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" t="s">
-        <v>98</v>
-      </c>
-      <c r="E16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" t="s">
-        <v>98</v>
-      </c>
-      <c r="G16" s="5">
-        <v>9.73</v>
-      </c>
-      <c r="H16" s="5">
-        <f t="shared" ref="H16:H28" si="2">B16*G16</f>
-        <v>9.73</v>
-      </c>
-      <c r="I16" t="s">
-        <v>97</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G17" s="5">
-        <v>0.01</v>
-      </c>
       <c r="H17" s="5">
         <f>B17*G17</f>
-        <v>0.01</v>
+        <v>11.661199999999999</v>
       </c>
       <c r="I17" t="s">
-        <v>28</v>
+        <v>105</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1451,424 +1486,487 @@
       <c r="C18" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>112</v>
+      <c r="D18" t="s">
+        <v>97</v>
       </c>
       <c r="E18" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G18" s="5">
+        <v>9.73</v>
+      </c>
+      <c r="H18" s="5">
+        <f t="shared" ref="H18:H30" si="2">B18*G18</f>
+        <v>9.73</v>
+      </c>
+      <c r="I18" t="s">
+        <v>96</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="H19" s="5">
+        <f>B19*G19</f>
+        <v>0.01</v>
+      </c>
+      <c r="I19" t="s">
+        <v>27</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
         <v>112</v>
       </c>
-      <c r="G18" s="9">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G20" s="9">
         <f>4.8/49</f>
         <v>9.7959183673469383E-2</v>
       </c>
-      <c r="H18" s="5">
-        <f t="shared" ref="H18:H19" si="3">B18*G18</f>
+      <c r="H20" s="5">
+        <f t="shared" ref="H20:H21" si="3">B20*G20</f>
         <v>9.7959183673469383E-2</v>
       </c>
-      <c r="I18" t="s">
-        <v>116</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>114</v>
-      </c>
-      <c r="B19">
+      <c r="I20" t="s">
+        <v>115</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21">
         <v>1</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C21" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="D21" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E21" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="G19" s="9">
+      <c r="F21" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G21" s="9">
         <f>4.8/49</f>
         <v>9.7959183673469383E-2</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H21" s="5">
         <f t="shared" si="3"/>
         <v>9.7959183673469383E-2</v>
       </c>
-      <c r="I19" t="s">
-        <v>115</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="I21" t="s">
+        <v>114</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B22" s="11">
         <v>1</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="D20" s="12" t="s">
+      <c r="C22" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="D22" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="E22" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="G20" s="13">
+      <c r="F22" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="G22" s="13">
         <v>0.58450000000000002</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H22" s="13">
         <f t="shared" si="2"/>
         <v>0.58450000000000002</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="I22" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="J22" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="J20" s="10" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="B21">
+      <c r="B23">
         <v>1</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C23" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E23" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G23" s="5">
         <v>0.90280000000000005</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H23" s="5">
         <f t="shared" si="2"/>
         <v>0.90280000000000005</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I23" t="s">
         <v>24</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="J23" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24">
         <v>1</v>
       </c>
-      <c r="C22" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" s="3" t="s">
+      <c r="C24" t="s">
         <v>34</v>
       </c>
-      <c r="E22" t="s">
+      <c r="D24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" s="5">
+      <c r="F24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G24" s="5">
         <v>0.53400000000000003</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H24" s="5">
         <f t="shared" si="2"/>
         <v>0.53400000000000003</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I24" t="s">
+        <v>35</v>
+      </c>
+      <c r="J24" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J22" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25">
         <v>1</v>
       </c>
-      <c r="C23" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="3" t="s">
+      <c r="C25" t="s">
         <v>39</v>
       </c>
-      <c r="E23" t="s">
+      <c r="D25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G23" s="5">
+      <c r="F25" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G25" s="5">
         <v>0.63229999999999997</v>
       </c>
-      <c r="H23" s="5">
+      <c r="H25" s="5">
         <f t="shared" si="2"/>
         <v>0.63229999999999997</v>
       </c>
-      <c r="I23" t="s">
-        <v>41</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="I25" t="s">
+        <v>40</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
         <v>47</v>
       </c>
-      <c r="B24">
-        <v>10</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="D26" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="E26" t="s">
         <v>19</v>
       </c>
-      <c r="F24" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G24" s="5">
+      <c r="F26" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G26" s="5">
         <v>3.0300000000000001E-2</v>
       </c>
-      <c r="H24" s="5">
+      <c r="H26" s="5">
         <f t="shared" si="2"/>
         <v>0.30299999999999999</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I26" t="s">
+        <v>49</v>
+      </c>
+      <c r="J26" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="J24" s="2" t="s">
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B25">
-        <v>2</v>
-      </c>
-      <c r="C25" t="s">
-        <v>48</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="E27" t="s">
         <v>19</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G25" s="5">
+      <c r="F27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="5">
         <v>3.8100000000000002E-2</v>
       </c>
-      <c r="H25" s="5">
+      <c r="H27" s="5">
         <f t="shared" si="2"/>
         <v>7.6200000000000004E-2</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I27" t="s">
+        <v>53</v>
+      </c>
+      <c r="J27" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="J25" s="2" t="s">
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="E28" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G26" s="5">
+      <c r="F28" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G28" s="5">
         <v>7.5899999999999995E-2</v>
       </c>
-      <c r="H26" s="5">
+      <c r="H28" s="5">
         <f t="shared" si="2"/>
         <v>7.5899999999999995E-2</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I28" t="s">
+        <v>57</v>
+      </c>
+      <c r="J28" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J26" s="2" t="s">
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-      <c r="C27" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="E29" t="s">
         <v>19</v>
       </c>
-      <c r="F27" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G27" s="5">
+      <c r="F29" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G29" s="5">
         <v>6.3799999999999996E-2</v>
       </c>
-      <c r="H27" s="5">
+      <c r="H29" s="5">
         <f t="shared" si="2"/>
         <v>0.12759999999999999</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I29" t="s">
+        <v>61</v>
+      </c>
+      <c r="J29" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J27" s="2" t="s">
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="D30" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="E30" t="s">
+        <v>63</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G28" s="5">
+      <c r="G30" s="5">
         <v>0.3871</v>
       </c>
-      <c r="H28" s="5">
+      <c r="H30" s="5">
         <f t="shared" si="2"/>
         <v>0.3871</v>
       </c>
-      <c r="I28" t="s">
-        <v>132</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G29" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H29" s="5">
-        <f>SUM(H2:H28)</f>
-        <v>44.462735034013583</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="I30" t="s">
+        <v>131</v>
+      </c>
+      <c r="J30" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G30" s="4"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="G31" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H31" s="5">
+        <f>SUM(H2:H30)</f>
+        <v>44.812335034013593</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J33" s="2"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="J35" s="2"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J21" r:id="rId1" xr:uid="{5EB9FB3D-22AD-47DC-B125-539430A9CC29}"/>
-    <hyperlink ref="J17" r:id="rId2" xr:uid="{53BAB52E-738A-40FD-AE11-30F4B5C07642}"/>
-    <hyperlink ref="J22" r:id="rId3" xr:uid="{D254588B-7BF2-4663-B764-31CEE1702B72}"/>
-    <hyperlink ref="J23" r:id="rId4" xr:uid="{97844978-768D-4AF2-9FC1-EA6B6AEA91A7}"/>
+    <hyperlink ref="J23" r:id="rId1" xr:uid="{5EB9FB3D-22AD-47DC-B125-539430A9CC29}"/>
+    <hyperlink ref="J19" r:id="rId2" xr:uid="{53BAB52E-738A-40FD-AE11-30F4B5C07642}"/>
+    <hyperlink ref="J24" r:id="rId3" xr:uid="{D254588B-7BF2-4663-B764-31CEE1702B72}"/>
+    <hyperlink ref="J25" r:id="rId4" xr:uid="{97844978-768D-4AF2-9FC1-EA6B6AEA91A7}"/>
     <hyperlink ref="J2" r:id="rId5" xr:uid="{A783C18C-5336-47D4-B91E-5A0D50EFD847}"/>
-    <hyperlink ref="J25" r:id="rId6" xr:uid="{DA2D5093-8FE6-45A4-BA10-918A48B82B08}"/>
-    <hyperlink ref="J24" r:id="rId7" xr:uid="{F70812B2-9C02-459F-B38C-705355029FE7}"/>
-    <hyperlink ref="J26" r:id="rId8" xr:uid="{3F47DA3C-1E53-444A-8898-B9EA85FBD647}"/>
-    <hyperlink ref="J27" r:id="rId9" xr:uid="{13709938-D199-4718-8973-2310F69E82EA}"/>
+    <hyperlink ref="J27" r:id="rId6" xr:uid="{DA2D5093-8FE6-45A4-BA10-918A48B82B08}"/>
+    <hyperlink ref="J26" r:id="rId7" xr:uid="{F70812B2-9C02-459F-B38C-705355029FE7}"/>
+    <hyperlink ref="J28" r:id="rId8" xr:uid="{3F47DA3C-1E53-444A-8898-B9EA85FBD647}"/>
+    <hyperlink ref="J29" r:id="rId9" xr:uid="{13709938-D199-4718-8973-2310F69E82EA}"/>
     <hyperlink ref="J6" r:id="rId10" xr:uid="{97C57276-2433-4923-8B77-CF1D09F8B548}"/>
     <hyperlink ref="J7" r:id="rId11" xr:uid="{FC24FC01-0AA7-4D5B-BEA8-DAA6380AC073}"/>
     <hyperlink ref="J8" r:id="rId12" xr:uid="{384DB0BE-F1AE-4448-80D7-0387BA330343}"/>
     <hyperlink ref="J4" r:id="rId13" xr:uid="{E60A837F-D0CD-4E15-8F80-70CC3A0226A6}"/>
     <hyperlink ref="J5" r:id="rId14" xr:uid="{4A829B53-4217-4F26-89B4-F106E6B544CD}"/>
-    <hyperlink ref="J16" r:id="rId15" xr:uid="{305F8F85-0874-4D1F-9E8A-6D0403800691}"/>
-    <hyperlink ref="K15" r:id="rId16" xr:uid="{E0DF6966-BBD6-4D0C-B6F6-D79BAA6169DB}"/>
+    <hyperlink ref="J18" r:id="rId15" xr:uid="{305F8F85-0874-4D1F-9E8A-6D0403800691}"/>
+    <hyperlink ref="K17" r:id="rId16" xr:uid="{E0DF6966-BBD6-4D0C-B6F6-D79BAA6169DB}"/>
     <hyperlink ref="J11" r:id="rId17" xr:uid="{9DC153CF-6A36-4F67-AFC5-22DD9E35702B}"/>
-    <hyperlink ref="J15" r:id="rId18" xr:uid="{AA52E67F-B095-4E7F-9662-B6B8C8564EF9}"/>
-    <hyperlink ref="J19" r:id="rId19" xr:uid="{4A1380DF-B3F7-4272-8054-E7C4BBA79028}"/>
-    <hyperlink ref="J18" r:id="rId20" xr:uid="{8C9B92D8-2E44-4B6A-B72A-0A081445CCF4}"/>
+    <hyperlink ref="J17" r:id="rId18" xr:uid="{AA52E67F-B095-4E7F-9662-B6B8C8564EF9}"/>
+    <hyperlink ref="J21" r:id="rId19" xr:uid="{4A1380DF-B3F7-4272-8054-E7C4BBA79028}"/>
+    <hyperlink ref="J20" r:id="rId20" xr:uid="{8C9B92D8-2E44-4B6A-B72A-0A081445CCF4}"/>
     <hyperlink ref="J13" r:id="rId21" xr:uid="{3FB67847-D385-4555-A810-A1F070CC4594}"/>
     <hyperlink ref="J14" r:id="rId22" xr:uid="{5A506C84-4FD5-4C15-9819-9ADA9D37E63C}"/>
-    <hyperlink ref="J20" r:id="rId23" xr:uid="{66DCDBD3-0A17-4F25-A19C-055A4209733C}"/>
-    <hyperlink ref="J28" r:id="rId24" xr:uid="{DEB2DF39-759A-4E16-A9AB-E96ECF63A544}"/>
+    <hyperlink ref="J22" r:id="rId23" xr:uid="{66DCDBD3-0A17-4F25-A19C-055A4209733C}"/>
+    <hyperlink ref="J30" r:id="rId24" xr:uid="{DEB2DF39-759A-4E16-A9AB-E96ECF63A544}"/>
     <hyperlink ref="J3" r:id="rId25" xr:uid="{A2771846-5465-4023-A9E5-D8F1D4061B69}"/>
     <hyperlink ref="J9" r:id="rId26" xr:uid="{B027D582-DB2E-46D9-8854-474EB0EBDFB0}"/>
     <hyperlink ref="J10" r:id="rId27" xr:uid="{F077A7B0-1644-4316-9D46-032403F3533F}"/>
     <hyperlink ref="J12" r:id="rId28" xr:uid="{06C67DAE-C4AF-4036-B24C-1BF0591900B9}"/>
+    <hyperlink ref="J16" r:id="rId29" xr:uid="{4896EEAB-4995-4048-A26C-8C537C275962}"/>
+    <hyperlink ref="J15" r:id="rId30" xr:uid="{0C39BD60-52F2-4A18-A06E-62DD28F8365E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId29"/>
+  <pageSetup orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>